<commit_message>
resolved conficts and merged
</commit_message>
<xml_diff>
--- a/DRO Dump Report.xlsx
+++ b/DRO Dump Report.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C47CF1-86E2-46EF-9C7F-17681818AC51}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{03F731CC-36F4-429B-BFB5-222C125DEE2F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="42">
   <si>
     <t>#</t>
   </si>
@@ -49,21 +49,81 @@
     <t>No</t>
   </si>
   <si>
+    <t>Arthritis</t>
+  </si>
+  <si>
+    <t>Ankylosing Spondylitis Arthritis Impact Measurement Scales 2 (AS-AIMS2)</t>
+  </si>
+  <si>
+    <t>Scoring Logic is missing</t>
+  </si>
+  <si>
+    <t>Arthritis Impact Measurement Scale 2 (AIMS2) -SF</t>
+  </si>
+  <si>
+    <t>Arthritis Impact Measurement Scale 2 (AIMS2)</t>
+  </si>
+  <si>
+    <t>Same as #2</t>
+  </si>
+  <si>
+    <t>Arthritis Impact Measurement Scale 2 (AIMS2)-SF reference</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>This is a reference document.</t>
+  </si>
+  <si>
+    <t>Back Pain Functional Scale (BPFS)</t>
+  </si>
+  <si>
+    <t>Back Pain</t>
+  </si>
+  <si>
+    <t>BASDAI</t>
+  </si>
+  <si>
+    <t>Pain</t>
+  </si>
+  <si>
+    <t>This DRO doc is incomplete.</t>
+  </si>
+  <si>
+    <t>Bath Ankylosing Spondylitis Funcitonal Index (BASFI)</t>
+  </si>
+  <si>
+    <t>Ankylosing Spondylitis</t>
+  </si>
+  <si>
+    <t>Scoring and Scoring Logic is missing</t>
+  </si>
+  <si>
+    <t>Bournemouth Questionnaire (BQ)</t>
+  </si>
+  <si>
+    <t>Childhood Asthma control test</t>
+  </si>
+  <si>
+    <t>Section (ACT in 12yr old teens) of this matches #1</t>
+  </si>
+  <si>
+    <t>Hospital Anxiety and Depression Scale (HADS)</t>
+  </si>
+  <si>
+    <t>Anxiety</t>
+  </si>
+  <si>
     <t>Childhood Asthma</t>
   </si>
   <si>
     <t>CIJSS</t>
   </si>
   <si>
-    <t>Arthritis</t>
-  </si>
-  <si>
     <t>DPQ</t>
   </si>
   <si>
-    <t>Pain</t>
-  </si>
-  <si>
     <t>DASH</t>
   </si>
   <si>
@@ -73,13 +133,13 @@
     <t>DHI</t>
   </si>
   <si>
+    <t>Handicap</t>
+  </si>
+  <si>
     <t>EORTC QLQ-C30</t>
   </si>
   <si>
     <t>Quality of life</t>
-  </si>
-  <si>
-    <t>Handicap</t>
   </si>
   <si>
     <t>EuroQol-5D (EQ-5D)</t>
@@ -98,12 +158,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -118,8 +184,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -129,28 +207,28 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -503,18 +581,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:G64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="2"/>
+    <col min="2" max="2" width="7.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14" style="2" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="28.5703125" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -555,215 +635,301 @@
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>2</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>3</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>4</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>5</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>6</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>7</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>8</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>9</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>10</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="1">
+      <c r="B15" s="5">
         <v>11</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="5">
+        <v>12</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="1" t="s">
+      <c r="E16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="1">
-        <v>12</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="5">
+        <v>13</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="1">
-        <v>13</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="1" t="s">
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="5">
         <v>14</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" s="1" t="s">
+      <c r="C18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="1">
-        <v>14</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="5">
         <v>15</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="C19" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="5">
         <v>16</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="1" t="s">
+      <c r="C20" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="1">
-        <v>15</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="5">
         <v>17</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="1">
-        <v>16</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="1">
-        <v>17</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
+      <c r="C21" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
@@ -895,12 +1061,16 @@
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B35" s="1">
         <v>31</v>
       </c>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
+      <c r="C35" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>

</xml_diff>